<commit_message>
Add RQ2 (Tinnitus Loudness) to evaluations
Also, add features importances for tinnitus loudness
</commit_message>
<xml_diff>
--- a/results/01_tables/ml_features_describe.xlsx
+++ b/results/01_tables/ml_features_describe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\tinnitus-country\results\01_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3497868C-5FB3-4ACC-A6D2-093BAEB8F460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BBD697-D12B-4360-BC6E-9A8FF7B71B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E76C60A-F1B8-4053-A971-514E6DE7161C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>mean</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>year_of_birth</t>
-  </si>
-  <si>
     <t>question4</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Year of birth</t>
-  </si>
-  <si>
     <t>How is your mood right now?</t>
   </si>
   <si>
@@ -174,10 +168,24 @@
     <t>scaling</t>
   </si>
   <si>
-    <t>SAM from 0 to 1 with stepsize 0.125</t>
-  </si>
-  <si>
-    <t>Slider in range (0, 1)</t>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Age in years</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>How loud is the tinnitus right now?</t>
+  </si>
+  <si>
+    <t>Slider in 
+range (0, 1)</t>
+  </si>
+  <si>
+    <t>SAM from 0 to 1
+with stepsize 0.125</t>
   </si>
 </sst>
 </file>
@@ -222,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -282,30 +290,6 @@
     <border>
       <left/>
       <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -356,11 +340,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -393,16 +408,43 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -411,47 +453,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC77EA5-F842-4AF6-93AB-94BBBD528839}">
-  <dimension ref="B1:F23"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,10 +815,10 @@
     <row r="1" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>0</v>
@@ -796,38 +826,38 @@
       <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>45</v>
+      <c r="F2" s="35" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="C3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14">
         <v>1.8220475375675501E-2</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="14">
         <v>0.133748424970285</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>43</v>
+      <c r="F3" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="22">
+      <c r="C4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="16">
         <v>2.5810222440577998E-2</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="16">
         <v>0.15856944172108201</v>
       </c>
       <c r="F4" s="23"/>
@@ -836,13 +866,13 @@
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="22">
+      <c r="C5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="16">
         <v>8.1852372643027693E-2</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="16">
         <v>0.27414083668020101</v>
       </c>
       <c r="F5" s="23"/>
@@ -851,13 +881,13 @@
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="C6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="16">
         <v>0.62097853524658198</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="16">
         <v>0.48514553252175302</v>
       </c>
       <c r="F6" s="23"/>
@@ -866,13 +896,13 @@
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="C7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="16">
         <v>4.7410507056092899E-2</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="16">
         <v>0.212516195712667</v>
       </c>
       <c r="F7" s="23"/>
@@ -881,13 +911,13 @@
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="22">
+      <c r="C8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="16">
         <v>1.08340251071543E-2</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="16">
         <v>0.10352168751231899</v>
       </c>
       <c r="F8" s="23"/>
@@ -896,13 +926,13 @@
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="22">
+      <c r="C9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16">
         <v>6.6960882308096298E-2</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="16">
         <v>0.24995529956020199</v>
       </c>
       <c r="F9" s="23"/>
@@ -911,13 +941,13 @@
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="22">
+      <c r="C10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="16">
         <v>1.6627983804021799E-2</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="16">
         <v>0.12787350182280799</v>
       </c>
       <c r="F10" s="23"/>
@@ -926,13 +956,13 @@
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="22">
+      <c r="C11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16">
         <v>1.97875548477815E-2</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="16">
         <v>0.13927013972831201</v>
       </c>
       <c r="F11" s="23"/>
@@ -941,13 +971,13 @@
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="22">
+      <c r="C12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="16">
         <v>9.1517441170989505E-2</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="16">
         <v>0.288344764838037</v>
       </c>
       <c r="F12" s="23"/>
@@ -956,13 +986,13 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="22">
+      <c r="C13" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="16">
         <v>0.256213258339404</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="16">
         <v>0.43654282590453902</v>
       </c>
       <c r="F13" s="23"/>
@@ -971,11 +1001,11 @@
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="22">
+      <c r="C14" s="27"/>
+      <c r="D14" s="16">
         <v>0.24034763752181201</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="16">
         <v>0.42729638105006901</v>
       </c>
       <c r="F14" s="23"/>
@@ -984,11 +1014,11 @@
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="22">
+      <c r="C15" s="27"/>
+      <c r="D15" s="16">
         <v>0.24896233926847</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="16">
         <v>0.43241377956779098</v>
       </c>
       <c r="F15" s="23"/>
@@ -997,11 +1027,11 @@
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="22">
+      <c r="C16" s="27"/>
+      <c r="D16" s="16">
         <v>0.25447676487031301</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="16">
         <v>0.43556853429992798</v>
       </c>
       <c r="F16" s="23"/>
@@ -1010,72 +1040,72 @@
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0.73604452199840698</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.44077730132270099</v>
+      </c>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="21">
+        <v>49.71</v>
+      </c>
+      <c r="E18" s="21">
+        <v>12.98</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="25">
-        <v>0.73604452199840698</v>
-      </c>
-      <c r="E17" s="25">
-        <v>0.44077730132270099</v>
-      </c>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="29">
-        <v>1967.84878106629</v>
-      </c>
-      <c r="E18" s="29">
-        <v>12.6842980453201</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="20">
+      <c r="D19" s="14">
         <v>0.57993746381332201</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="14">
         <v>0.204040000634364</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>46</v>
+      <c r="F19" s="22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="25">
+        <v>18</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="18">
         <v>0.247334524878395</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="18">
         <v>0.21795589473798699</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D21" s="8">
         <v>0.25616444567727698</v>
@@ -1083,16 +1113,16 @@
       <c r="E21" s="8">
         <v>0.23000862943688499</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>47</v>
+      <c r="F21" s="25" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="11">
         <v>0.58720455238413805</v>
@@ -1100,24 +1130,44 @@
       <c r="E22" s="11">
         <v>0.31267809607147601</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="2:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="13">
+      <c r="B23" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="32">
         <v>0.5</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="32">
         <v>0.50000211768841596</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="F23" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.47</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>